<commit_message>
DB_Memory: Latest update on PCB checklist and waiting for final revision of v1.1 realease
</commit_message>
<xml_diff>
--- a/Memory_Expansion_Daughter_Board/hardware/PCB Design Checklist.xlsx
+++ b/Memory_Expansion_Daughter_Board/hardware/PCB Design Checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\daughter_boards_obdh2\Memory_Expansion_Daughter_Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\daughter_boards_obdh2\Memory_Expansion_Daughter_Board\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B256F4-B66D-4B60-95A6-348A9EA4A9A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D6FC47-2008-4355-9675-C9B92CC9AAA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="178">
   <si>
     <t>1.</t>
   </si>
@@ -476,15 +476,9 @@
     <t>4.3</t>
   </si>
   <si>
-    <t>Project: Memory Daughter Board OBDH 2.0 FloripaSat-2</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
-    <t>Using GPIO 4</t>
-  </si>
-  <si>
     <t>Variant: 1.0</t>
   </si>
   <si>
@@ -506,15 +500,9 @@
     <t>Excel sheet done by Kleber Reis Gouveia Júnior, Electronic Engineer, source: https://kleberrgouveia.wixsite.com/home/goodstuff</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>Used lower values of capacitance due to project aplication.</t>
   </si>
   <si>
-    <t>Added to "POWER TEST" pin connector</t>
-  </si>
-  <si>
     <t>Not needed?</t>
   </si>
   <si>
@@ -558,6 +546,27 @@
   </si>
   <si>
     <t>too large table and it is not know how to resize it</t>
+  </si>
+  <si>
+    <t>Dual suply not necessary.</t>
+  </si>
+  <si>
+    <t>Using GPIO 4.</t>
+  </si>
+  <si>
+    <t>Added to "POWER TEST" pin connector.</t>
+  </si>
+  <si>
+    <t>Gabriel Mariano Marcelino</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Project: Memory Expansion Daughter Board of OBDH 2.0 ALT Hardware</t>
+  </si>
+  <si>
+    <t>In a unified PDF containing layer prints, assembly drawings and BOM.</t>
   </si>
 </sst>
 </file>
@@ -617,7 +626,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,6 +647,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -716,7 +731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -800,6 +815,16 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Ênfase1" xfId="1" builtinId="29"/>
@@ -807,6 +832,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1120,8 +1150,8 @@
   </sheetPr>
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,7 +1164,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -1154,7 +1184,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -1162,13 +1192,13 @@
         <v>68</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>157</v>
+        <v>1</v>
       </c>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -1177,7 +1207,7 @@
       </c>
       <c r="E4" s="9">
         <f ca="1">NOW()</f>
-        <v>43887.794990972223</v>
+        <v>43914.033173958334</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1224,7 +1254,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="7" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1254,21 +1284,21 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="7" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="7" t="s">
-        <v>148</v>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1278,11 +1308,13 @@
       <c r="B11" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="7" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1336,10 +1368,10 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="E15" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -1348,12 +1380,12 @@
       <c r="B16" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -1368,7 +1400,7 @@
         <v>134</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1384,21 +1416,21 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="7" t="s">
-        <v>148</v>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1414,21 +1446,21 @@
         <v>134</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="7" t="s">
-        <v>148</v>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1516,7 +1548,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1546,7 +1578,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1560,7 +1592,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1576,21 +1608,21 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="7" t="s">
-        <v>148</v>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1604,7 +1636,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1662,21 +1694,21 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="7" t="s">
-        <v>148</v>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1692,7 +1724,7 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1708,7 +1740,7 @@
         <v>134</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1724,35 +1756,35 @@
         <v>134</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="7" t="s">
-        <v>148</v>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="7" t="s">
-        <v>148</v>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1770,18 +1802,16 @@
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="32"/>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
@@ -1796,7 +1826,7 @@
         <v>134</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1810,7 +1840,7 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1824,21 +1854,21 @@
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="7" t="s">
-        <v>148</v>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1890,23 +1920,25 @@
       <c r="B53" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="7" t="s">
-        <v>148</v>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1918,23 +1950,23 @@
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="E55" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F55" s="7"/>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="7" t="s">
-        <v>148</v>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1946,9 +1978,11 @@
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="F57" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1966,17 +2000,17 @@
       <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="7" t="s">
-        <v>148</v>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1992,21 +2026,21 @@
         <v>134</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="7" t="s">
-        <v>148</v>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2046,7 +2080,9 @@
       <c r="B64" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C64" s="2"/>
+      <c r="C64" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D64" s="1"/>
       <c r="E64" s="2"/>
       <c r="F64" s="3"/>
@@ -2058,7 +2094,9 @@
       <c r="B65" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C65" s="2"/>
+      <c r="C65" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D65" s="1"/>
       <c r="E65" s="2"/>
       <c r="F65" s="3"/>
@@ -2072,7 +2110,9 @@
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="2"/>
+      <c r="E66" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2082,10 +2122,14 @@
       <c r="B67" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C67" s="2"/>
+      <c r="C67" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D67" s="1"/>
       <c r="E67" s="2"/>
-      <c r="F67" s="3"/>
+      <c r="F67" s="3" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
@@ -2094,7 +2138,9 @@
       <c r="B68" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C68" s="2"/>
+      <c r="C68" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D68" s="1"/>
       <c r="E68" s="2"/>
       <c r="F68" s="3"/>
@@ -2106,7 +2152,9 @@
       <c r="B69" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C69" s="2"/>
+      <c r="C69" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D69" s="1"/>
       <c r="E69" s="2"/>
       <c r="F69" s="3"/>
@@ -2118,7 +2166,9 @@
       <c r="B70" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C70" s="2"/>
+      <c r="C70" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D70" s="1"/>
       <c r="E70" s="2"/>
       <c r="F70" s="3"/>
@@ -2144,7 +2194,9 @@
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="1"/>
-      <c r="E72" s="2"/>
+      <c r="E72" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2178,10 +2230,10 @@
         <v>136</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D75" s="18"/>
       <c r="E75" s="19"/>
@@ -2192,10 +2244,10 @@
         <v>137</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D76" s="18"/>
       <c r="E76" s="19"/>
@@ -2206,10 +2258,10 @@
         <v>146</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="19"/>
@@ -2217,11 +2269,13 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B78" s="10"/>
+        <v>163</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>153</v>
+      </c>
       <c r="C78" s="17" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="D78" s="18"/>
       <c r="E78" s="19"/>
@@ -2229,12 +2283,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B79" s="10"/>
-      <c r="C79" s="17" t="s">
-        <v>154</v>
-      </c>
+      <c r="C79" s="17"/>
       <c r="D79" s="18"/>
       <c r="E79" s="19"/>
       <c r="F79" s="14"/>

</xml_diff>

<commit_message>
DB_Memory: Finished PCB Design Checklist
</commit_message>
<xml_diff>
--- a/Memory_Expansion_Daughter_Board/hardware/PCB Design Checklist.xlsx
+++ b/Memory_Expansion_Daughter_Board/hardware/PCB Design Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\daughter_boards_obdh2\Memory_Expansion_Daughter_Board\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D6FC47-2008-4355-9675-C9B92CC9AAA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930C65C2-EB41-49B8-BD11-11BA835A7169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
+    <workbookView xWindow="-28920" yWindow="-3645" windowWidth="29040" windowHeight="15840" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="180">
   <si>
     <t>1.</t>
   </si>
@@ -476,9 +476,6 @@
     <t>4.3</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Variant: 1.0</t>
   </si>
   <si>
@@ -503,9 +500,6 @@
     <t>Used lower values of capacitance due to project aplication.</t>
   </si>
   <si>
-    <t>Not needed?</t>
-  </si>
-  <si>
     <t>Same default thickness of OBDH 2.0</t>
   </si>
   <si>
@@ -515,9 +509,6 @@
     <t>No polarity components on project.</t>
   </si>
   <si>
-    <t>Daughter Board PCB holes are standard for any aplication.</t>
-  </si>
-  <si>
     <t>FSI connector has 1.07 mm diameter alligment pin (AD version).</t>
   </si>
   <si>
@@ -527,27 +518,12 @@
     <t>4.4</t>
   </si>
   <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>Still needs final revision, some may not be acording to standard</t>
-  </si>
-  <si>
-    <t>Power width of 0.508mm and all other tracks with 0.254mm?</t>
-  </si>
-  <si>
     <t>Not a high speed design</t>
   </si>
   <si>
     <t>Simple design that doesn't require it</t>
   </si>
   <si>
-    <t>Initial placement but is not showing hole in drill drawing layer</t>
-  </si>
-  <si>
-    <t>too large table and it is not know how to resize it</t>
-  </si>
-  <si>
     <t>Dual suply not necessary.</t>
   </si>
   <si>
@@ -560,13 +536,43 @@
     <t>Gabriel Mariano Marcelino</t>
   </si>
   <si>
-    <t>Support</t>
-  </si>
-  <si>
     <t>Project: Memory Expansion Daughter Board of OBDH 2.0 ALT Hardware</t>
   </si>
   <si>
     <t>In a unified PDF containing layer prints, assembly drawings and BOM.</t>
+  </si>
+  <si>
+    <t>Only used extra capacitors on daughter board, ODBH 2.0 has ferrite breads and capacitors covered</t>
+  </si>
+  <si>
+    <t>Provided by mother board (OBDH 2.0) with a 1M ohm resistor connected to the structure</t>
+  </si>
+  <si>
+    <t>Daughter Board PCB holes are standard for any variation.</t>
+  </si>
+  <si>
+    <t>Power width of 0.508mm and all other tracks with 0.254mm (following standard of motherboard)</t>
+  </si>
+  <si>
+    <t>This simple board design doesn't need it</t>
+  </si>
+  <si>
+    <t>No 90 degre tracks in pcb design</t>
+  </si>
+  <si>
+    <t>Too large table and it is not yet know how to resize it in Altium 18.1.7</t>
+  </si>
+  <si>
+    <t>Only GND vias used in this simple 2 layer design</t>
+  </si>
+  <si>
+    <t>Only ESD silk added</t>
+  </si>
+  <si>
+    <t>X*</t>
+  </si>
+  <si>
+    <t>*Only the FSI connector needing special revision for mating pads, no source found yet</t>
   </si>
 </sst>
 </file>
@@ -626,7 +632,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -650,14 +656,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -726,12 +726,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -779,6 +805,33 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -797,34 +850,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Ênfase1" xfId="1" builtinId="29"/>
@@ -1148,10 +1176,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,55 +1187,55 @@
     <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.28515625" customWidth="1"/>
+    <col min="6" max="6" width="91.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="A1" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="A3" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
+      <c r="A4" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="7" t="s">
         <v>69</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">NOW()</f>
-        <v>43914.033173958334</v>
+        <v>43940.990319328703</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1215,19 +1243,19 @@
       <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="15" t="s">
         <v>63</v>
       </c>
@@ -1254,7 +1282,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="7" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1284,22 +1312,22 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="7" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32" t="s">
-        <v>147</v>
-      </c>
+      <c r="C10" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -1314,7 +1342,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="7" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1400,7 +1428,7 @@
         <v>134</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1415,52 +1443,56 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="7" t="s">
-        <v>155</v>
+      <c r="F18" s="21" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32" t="s">
-        <v>147</v>
+      <c r="C19" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="18" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>156</v>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32" t="s">
-        <v>147</v>
+      <c r="C21" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1495,19 +1527,19 @@
       <c r="A24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="25"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="15" t="s">
         <v>63</v>
       </c>
@@ -1548,7 +1580,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1578,21 +1610,23 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="7" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="7" t="s">
-        <v>165</v>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="18" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1608,22 +1642,22 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="32" t="s">
-        <v>147</v>
-      </c>
+      <c r="C32" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
@@ -1632,11 +1666,13 @@
       <c r="B33" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="7" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1694,21 +1730,23 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="32" t="s">
-        <v>147</v>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1724,7 +1762,7 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1740,7 +1778,7 @@
         <v>134</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1756,36 +1794,38 @@
         <v>134</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="32" t="s">
-        <v>147</v>
+      <c r="C42" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="18" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="32" t="s">
-        <v>147</v>
-      </c>
+      <c r="C43" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="18"/>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
@@ -1802,16 +1842,18 @@
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="32"/>
+      <c r="C45" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="18"/>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
@@ -1826,7 +1868,7 @@
         <v>134</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1836,11 +1878,13 @@
       <c r="B47" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C47" s="2"/>
+      <c r="C47" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="7" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1850,25 +1894,27 @@
       <c r="B48" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="7" t="s">
-        <v>169</v>
-      </c>
+      <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="32" t="s">
-        <v>147</v>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E49" s="17"/>
+      <c r="F49" s="18" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1928,17 +1974,19 @@
       <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="29" t="s">
+      <c r="A54" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="32" t="s">
-        <v>147</v>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1948,26 +1996,28 @@
       <c r="B55" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D55" s="2"/>
-      <c r="E55" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F55" s="7"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="7" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B56" s="30" t="s">
+      <c r="B56" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="32" t="s">
-        <v>147</v>
-      </c>
+      <c r="C56" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="18"/>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
@@ -1982,7 +2032,7 @@
         <v>134</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2000,66 +2050,64 @@
       <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="29" t="s">
+      <c r="A59" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="30" t="s">
+      <c r="B59" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="32" t="s">
-        <v>147</v>
-      </c>
+      <c r="C59" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="18"/>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>168</v>
-      </c>
+      <c r="C60" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="18"/>
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="s">
+      <c r="A61" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="30" t="s">
+      <c r="B61" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="31"/>
-      <c r="F61" s="32" t="s">
-        <v>147</v>
-      </c>
+      <c r="C61" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="18"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="23" t="s">
+      <c r="B62" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C62" s="23"/>
-      <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="25" t="s">
+      <c r="A63" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="25"/>
+      <c r="B63" s="23"/>
       <c r="C63" s="15" t="s">
         <v>63</v>
       </c>
@@ -2128,7 +2176,7 @@
       <c r="D67" s="1"/>
       <c r="E67" s="2"/>
       <c r="F67" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2180,7 +2228,9 @@
       <c r="B71" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C71" s="2"/>
+      <c r="C71" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D71" s="1"/>
       <c r="E71" s="2"/>
       <c r="F71" s="3"/>
@@ -2203,24 +2253,24 @@
       <c r="A73" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B73" s="23" t="s">
+      <c r="B73" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="24" t="s">
+      <c r="A74" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="24"/>
-      <c r="C74" s="26" t="s">
+      <c r="B74" s="34"/>
+      <c r="C74" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="27"/>
-      <c r="E74" s="28"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="27"/>
       <c r="F74" s="16" t="s">
         <v>75</v>
       </c>
@@ -2230,13 +2280,13 @@
         <v>136</v>
       </c>
       <c r="B75" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C75" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="C75" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D75" s="18"/>
-      <c r="E75" s="19"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="30"/>
       <c r="F75" s="14"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2244,13 +2294,13 @@
         <v>137</v>
       </c>
       <c r="B76" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C76" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="C76" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D76" s="18"/>
-      <c r="E76" s="19"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="30"/>
       <c r="F76" s="14"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2258,45 +2308,31 @@
         <v>146</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D77" s="18"/>
-      <c r="E77" s="19"/>
+        <v>166</v>
+      </c>
+      <c r="C77" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D77" s="29"/>
+      <c r="E77" s="30"/>
       <c r="F77" s="14"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C78" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D78" s="18"/>
-      <c r="E78" s="19"/>
+        <v>152</v>
+      </c>
+      <c r="C78" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D78" s="29"/>
+      <c r="E78" s="30"/>
       <c r="F78" s="14"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B79" s="10"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="19"/>
-      <c r="F79" s="14"/>
-    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C79:E79"/>
+  <mergeCells count="17">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C75:E75"/>
     <mergeCell ref="C76:E76"/>
@@ -2311,6 +2347,9 @@
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="B5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C78:E78"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>